<commit_message>
various improvements to game loop
</commit_message>
<xml_diff>
--- a/DungeonGame/res/item/ItemList.xlsx
+++ b/DungeonGame/res/item/ItemList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Rainfall\DungeonGame\res\item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541D3C6-75DD-40E1-B39F-BFB71D7C25B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F621314B-958A-4DCC-A98D-F64AF284C005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CEF6D868-162A-445B-9C3D-56B2F4A2EFBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CEF6D868-162A-445B-9C3D-56B2F4A2EFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Cell Key</t>
+  </si>
+  <si>
+    <t>Broken Sword</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -161,7 +164,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -457,25 +460,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7251E18C-04C1-4EE9-95D5-E6A2FFCB2A48}">
-  <dimension ref="B1:X12"/>
+  <dimension ref="B1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" customWidth="1"/>
-    <col min="20" max="20" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -504,7 +507,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -554,7 +557,7 @@
         <v>6001</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -574,7 +577,7 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -588,7 +591,7 @@
         <v>4003</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -596,7 +599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -604,7 +607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -612,19 +615,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lots of stuff. level textures, hand spells, fireball spell, viewmodel overhaul, moveset improvements, resource folders improvements, voxel types with textures and properties, imgui beginnings
</commit_message>
<xml_diff>
--- a/DungeonGame/res/item/ItemList.xlsx
+++ b/DungeonGame/res/item/ItemList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Rainfall\DungeonGame\res\item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E1BF82-BD35-4B05-90CB-C06DBF3CBFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19982528-A014-42D4-BAE2-71CFD82459D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CEF6D868-162A-445B-9C3D-56B2F4A2EFBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CEF6D868-162A-445B-9C3D-56B2F4A2EFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Debug Weapon</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Iron Key</t>
+  </si>
+  <si>
+    <t>Fireball</t>
   </si>
 </sst>
 </file>
@@ -151,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -167,7 +176,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -463,25 +472,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7251E18C-04C1-4EE9-95D5-E6A2FFCB2A48}">
-  <dimension ref="B1:X14"/>
+  <dimension ref="B1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" customWidth="1"/>
-    <col min="20" max="20" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -509,8 +518,11 @@
       <c r="W1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Z1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -559,8 +571,14 @@
       <c r="X3">
         <v>6001</v>
       </c>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Z3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3">
+        <v>7001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -580,7 +598,7 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -594,15 +612,21 @@
         <v>4003</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -610,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -618,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -626,7 +650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -634,7 +658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -642,7 +666,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>

</xml_diff>